<commit_message>
lots of update, mainly rename
</commit_message>
<xml_diff>
--- a/Coba2.xlsx
+++ b/Coba2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="POSresults" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,9 @@
     <sheet name="Sheet4" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="CompilePref" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Sheet8" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="204">
   <si>
     <t xml:space="preserve">Embedding</t>
   </si>
@@ -347,12 +350,21 @@
     <t xml:space="preserve">Batch 12</t>
   </si>
   <si>
+    <t xml:space="preserve">A quarter of training data</t>
+  </si>
+  <si>
     <t xml:space="preserve">F-1 without O</t>
   </si>
   <si>
     <t xml:space="preserve">              precision    recall  f1-score   support</t>
   </si>
   <si>
+    <t xml:space="preserve">one eighth of training data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seed: 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">           O       0.99      0.92      0.95      9004</t>
   </si>
   <si>
@@ -374,10 +386,259 @@
     <t xml:space="preserve"> avg / total       0.95      0.90      0.92     10550</t>
   </si>
   <si>
+    <t xml:space="preserve">With POS Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With POS index &amp; add new training OOV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^ without weighting..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           O       0.98      0.93      0.95      9004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           O       0.99      0.93      0.96      9004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORGANIZATION       0.50      0.82      0.62       323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORGANIZATION       0.49      0.89      0.63       323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      PERSON       0.87      0.75      0.81       684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      PERSON       0.86      0.81      0.83       684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        TIME       0.85      0.80      0.82       287</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        TIME       0.82      0.84      0.83       287</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    LOCATION       0.73      0.67      0.70       213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    LOCATION       0.78      0.76      0.77       213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    QUANTITY       0.48      0.59      0.53        39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    QUANTITY       0.40      0.69      0.50        39</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> avg / total       0.95      0.91      0.93     10550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-1 Score (without O):</t>
+  </si>
+  <si>
     <t xml:space="preserve">Optimizer</t>
   </si>
   <si>
     <t xml:space="preserve">Loss Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prec &lt; recall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prec &gt; recall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batch 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01 loss delta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Without transfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With transfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 epoch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">518 s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 epoch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">730 s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 epoch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">587 s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No transfer No weighting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer No weighting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batch 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           O       0.98      0.96      0.97      7546</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      PERSON       0.94      0.80      0.86       653</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      PERSON       0.93      0.81      0.86       653</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORGANIZATION       0.76      0.66      0.71       367</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORGANIZATION       0.64      0.73      0.68       367</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    LOCATION       0.90      0.81      0.86       487</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    LOCATION       0.92      0.72      0.81       487</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> avg / total       0.96      0.93      0.95      9053</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> avg / total       0.96      0.93      0.94      9053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           O       0.98      0.92      0.95      9004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           O       0.99      0.90      0.94      9004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORGANIZATION       0.44      0.89      0.59       323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORGANIZATION       0.37      0.93      0.52       323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      PERSON       0.85      0.81      0.83       684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        TIME       0.85      0.79      0.82       287</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    LOCATION       0.74      0.68      0.71       213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    LOCATION       0.73      0.73      0.73       213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    QUANTITY       0.49      0.64      0.56        39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    QUANTITY       0.35      0.72      0.47        39</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> avg / total       0.95      0.89      0.91     10550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             precision    recall  f1-score   support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            precision    recall  f1-score   support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          O       0.97      0.97      0.97      7318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          O       0.98      0.96      0.97      7318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      B-PER       0.89      0.82      0.86       438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      B-PER       0.89      0.82      0.85       438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      I-PER       0.88      0.65      0.75       214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      I-PER       0.87      0.65      0.74       214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      B-ORG       0.72      0.74      0.73       296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      B-ORG       0.68      0.71      0.69       296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      I-ORG       0.53      0.65      0.59       151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      I-ORG       0.36      0.60      0.45       151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      B-LOC       0.74      0.73      0.74       218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      B-LOC       0.72      0.74      0.73       218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      I-LOC       0.67      0.78      0.72       141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      I-LOC       0.69      0.70      0.69       141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     B-MISC       0.61      0.08      0.14       141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     B-MISC       0.37      0.08      0.13       141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     I-MISC       0.54      0.16      0.25       154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     I-MISC       0.39      0.12      0.18       154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg / total       0.93      0.90      0.91      9071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg / total       0.92      0.90      0.91      9071</t>
   </si>
 </sst>
 </file>
@@ -715,6 +976,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
@@ -2020,22 +2284,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2360,7 +2624,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2674,17 +2938,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:K20"/>
+  <dimension ref="B1:N41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M44" activeCellId="0" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="9.71938775510204"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="N1" s="0"/>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
         <v>102</v>
@@ -2692,102 +2964,346 @@
       <c r="D2" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="E2" s="0"/>
+      <c r="H2" s="0"/>
       <c r="K2" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="N2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0"/>
       <c r="D3" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="E3" s="0"/>
+      <c r="H3" s="0"/>
       <c r="K3" s="21" t="n">
         <v>0.7213</v>
       </c>
+      <c r="N3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="N4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="N5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="H6" s="0"/>
+      <c r="K6" s="0"/>
+      <c r="N6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="K7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="N7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>107</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="K8" s="21" t="n">
+        <v>0.6809</v>
+      </c>
+      <c r="N8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="21" t="n">
         <v>0.7367</v>
       </c>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="K9" s="0"/>
+      <c r="N9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0"/>
+      <c r="D10" s="0"/>
+      <c r="E10" s="0"/>
+      <c r="H10" s="0"/>
+      <c r="K10" s="0"/>
+      <c r="N10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0"/>
+      <c r="D11" s="0"/>
       <c r="E11" s="22" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="H11" s="0"/>
+      <c r="K11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0"/>
+      <c r="D12" s="0"/>
       <c r="E12" s="22"/>
+      <c r="H12" s="0"/>
+      <c r="K12" s="21" t="n">
+        <v>0.5434</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0"/>
+      <c r="D13" s="0"/>
       <c r="E13" s="22" t="s">
-        <v>109</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="H13" s="0"/>
+      <c r="K13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0"/>
+      <c r="D14" s="0"/>
       <c r="E14" s="22" t="s">
-        <v>110</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="H14" s="0"/>
+      <c r="K14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0"/>
+      <c r="D15" s="0"/>
       <c r="E15" s="22" t="s">
-        <v>111</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="H15" s="0"/>
+      <c r="K15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0"/>
+      <c r="D16" s="0"/>
       <c r="E16" s="22" t="s">
-        <v>112</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="H16" s="0"/>
+      <c r="K16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0"/>
+      <c r="D17" s="0"/>
       <c r="E17" s="22" t="s">
-        <v>113</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="H17" s="0"/>
+      <c r="K17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0"/>
+      <c r="D18" s="0"/>
       <c r="E18" s="22" t="s">
-        <v>114</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="H18" s="0"/>
+      <c r="K18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0"/>
+      <c r="D19" s="0"/>
       <c r="E19" s="22"/>
+      <c r="H19" s="0"/>
+      <c r="K19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0"/>
+      <c r="D20" s="0"/>
       <c r="E20" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
+      </c>
+      <c r="H20" s="0"/>
+      <c r="K20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="H21" s="0"/>
+      <c r="K21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0"/>
+      <c r="D22" s="0"/>
+      <c r="E22" s="0"/>
+      <c r="H22" s="0"/>
+      <c r="K22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0"/>
+      <c r="D23" s="0"/>
+      <c r="E23" s="0"/>
+      <c r="H23" s="0"/>
+      <c r="K23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0"/>
+      <c r="D24" s="0"/>
+      <c r="E24" s="0"/>
+      <c r="H24" s="0"/>
+      <c r="K24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0"/>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="H25" s="0"/>
+      <c r="K25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="0"/>
+      <c r="H26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="21" t="n">
+        <v>0.738</v>
+      </c>
+      <c r="E27" s="0"/>
+      <c r="H27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="0"/>
+      <c r="H28" s="0"/>
+      <c r="K28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H29" s="0"/>
+      <c r="K29" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="22"/>
+      <c r="H30" s="0"/>
+      <c r="K30" s="22"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="H31" s="0"/>
+      <c r="K31" s="22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="H32" s="0"/>
+      <c r="K32" s="22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H33" s="0"/>
+      <c r="K33" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="H34" s="0"/>
+      <c r="K34" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="H35" s="0"/>
+      <c r="K35" s="22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="H36" s="0"/>
+      <c r="K36" s="22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="22"/>
+      <c r="H37" s="0"/>
+      <c r="K37" s="22"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="H38" s="0"/>
+      <c r="K38" s="22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H40" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H41" s="1" t="n">
+        <v>0.759880239521</v>
       </c>
     </row>
   </sheetData>
@@ -2814,14 +3330,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0"/>
       <c r="B1" s="0"/>
       <c r="C1" s="6" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -2857,7 +3373,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>15</v>
@@ -2876,4 +3392,526 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:I7"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.591490593342981</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.394327062228654</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">ROUND(AVERAGE(D3:E3),2)</f>
+        <v>0.49</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>4.74979662986636</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>3.16653108657757</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">ROUND(AVERAGE(D4:E4),2)</f>
+        <v>3.96</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>3.27894103489771</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2.95104693140794</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">ROUND(AVERAGE(D5:E5),2)</f>
+        <v>3.11</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1.75667621776504</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1.5614899713467</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">ROUND(AVERAGE(D6:E6),2)</f>
+        <v>1.66</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.442696994313566</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.221348497156783</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">ROUND(AVERAGE(D7:E7),2)</f>
+        <v>0.33</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L34"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="22"/>
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="H8" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="L8" s="22"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>0.822905620361</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0.799026425591</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="22"/>
+      <c r="L12" s="22"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F14" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="L14" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="L15" s="22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="L16" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="L17" s="22" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="L18" s="22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="H19" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="L19" s="22"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="n">
+        <v>0.738323353293</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0.707683741648</v>
+      </c>
+      <c r="L20" s="22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="L22" s="22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23" s="22"/>
+      <c r="L23" s="22"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F24" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="L24" s="22" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F25" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="L25" s="22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F26" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="L26" s="22" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F27" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="L27" s="22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F28" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="L28" s="22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F29" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="L29" s="22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F30" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="L30" s="22" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F31" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="L31" s="22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F32" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="L32" s="22" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="F33" s="22"/>
+      <c r="H33" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="L33" s="22"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="n">
+        <v>0.692118226601</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>0.654391789919</v>
+      </c>
+      <c r="L34" s="22" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update pos experiment autos
</commit_message>
<xml_diff>
--- a/Coba2.xlsx
+++ b/Coba2.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="259">
   <si>
     <t xml:space="preserve">Embedding</t>
   </si>
@@ -748,22 +748,37 @@
     <t xml:space="preserve">Embedding (word &amp; char)</t>
   </si>
   <si>
+    <t xml:space="preserve">auto_script.sh</t>
+  </si>
+  <si>
     <t xml:space="preserve">Model (WE/CE/Both)</t>
   </si>
   <si>
     <t xml:space="preserve">Trainable Embedding</t>
   </si>
   <si>
+    <t xml:space="preserve">← using best embedding; no trainable only, trainable data are get from previous experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auto_script_notrain.sh</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bidirectional merge (char)</t>
   </si>
   <si>
     <t xml:space="preserve">← model CE</t>
   </si>
   <si>
+    <t xml:space="preserve">auto_script_ce.sh</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bidirectional merge (word)</t>
   </si>
   <si>
     <t xml:space="preserve">← model WE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auto_script_we.sh</t>
   </si>
   <si>
     <t xml:space="preserve">Merging layer</t>
@@ -802,7 +817,7 @@
     <numFmt numFmtId="165" formatCode="0.00%"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -850,6 +865,13 @@
     </font>
     <font>
       <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -982,7 +1004,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1087,11 +1109,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1167,7 +1193,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart148.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1609,11 +1635,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="44684170"/>
-        <c:axId val="22410993"/>
+        <c:axId val="24434116"/>
+        <c:axId val="59376137"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44684170"/>
+        <c:axId val="24434116"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1648,14 +1674,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22410993"/>
+        <c:crossAx val="59376137"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22410993"/>
+        <c:axId val="59376137"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1699,7 +1725,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44684170"/>
+        <c:crossAx val="24434116"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1736,7 +1762,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart149.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4264,11 +4290,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="72964591"/>
-        <c:axId val="71480532"/>
+        <c:axId val="33072852"/>
+        <c:axId val="92912983"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72964591"/>
+        <c:axId val="33072852"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4303,14 +4329,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71480532"/>
+        <c:crossAx val="92912983"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71480532"/>
+        <c:axId val="92912983"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4354,7 +4380,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72964591"/>
+        <c:crossAx val="33072852"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4391,7 +4417,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart150.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4627,11 +4653,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="49038381"/>
-        <c:axId val="96294575"/>
+        <c:axId val="67022188"/>
+        <c:axId val="81346848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49038381"/>
+        <c:axId val="67022188"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4666,14 +4692,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96294575"/>
+        <c:crossAx val="81346848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96294575"/>
+        <c:axId val="81346848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4717,7 +4743,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49038381"/>
+        <c:crossAx val="67022188"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4765,9 +4791,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>561960</xdr:colOff>
+      <xdr:colOff>561600</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4775,8 +4801,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3157560" y="361080"/>
-        <a:ext cx="5671800" cy="3237840"/>
+        <a:off x="3109680" y="361080"/>
+        <a:ext cx="5586120" cy="3237480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4795,9 +4821,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>463680</xdr:colOff>
+      <xdr:colOff>463320</xdr:colOff>
       <xdr:row>248</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>96840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4806,7 +4832,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="107280" y="36373320"/>
-        <a:ext cx="18072720" cy="4486320"/>
+        <a:ext cx="17786520" cy="4485960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4830,9 +4856,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>86400</xdr:colOff>
+      <xdr:colOff>86040</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4840,8 +4866,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3019320" y="6032880"/>
-        <a:ext cx="4267800" cy="3237120"/>
+        <a:off x="2971800" y="6032880"/>
+        <a:ext cx="4200840" cy="3236760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4866,9 +4892,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
@@ -6169,12 +6192,12 @@
   <dimension ref="B2:K31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6192,15 +6215,18 @@
         <v>238</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>3</v>
@@ -6208,59 +6234,71 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>242</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="26" t="s">
-        <v>241</v>
-      </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26" t="s">
-        <v>242</v>
-      </c>
-      <c r="E12" s="26" t="n">
+      <c r="B12" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="E12" s="27" t="n">
         <v>3</v>
       </c>
       <c r="F12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="E14" s="27" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="26" t="s">
-        <v>243</v>
-      </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26" t="s">
-        <v>244</v>
-      </c>
-      <c r="E14" s="26" t="n">
-        <v>3</v>
-      </c>
       <c r="F14" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>5</v>
@@ -6271,7 +6309,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>8</v>
@@ -6282,7 +6320,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>14</v>
@@ -6291,17 +6329,17 @@
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F20" s="0" t="n">
         <f aca="false">SUM(F6:F18)</f>
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="25" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="27" t="s">
-        <v>250</v>
+      <c r="B23" s="28" t="s">
+        <v>255</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>148</v>
@@ -6312,7 +6350,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>1</v>
@@ -6321,7 +6359,7 @@
         <v>4</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="K25" s="0" t="n">
         <v>1</v>
@@ -6335,7 +6373,7 @@
         <v>8</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="K27" s="0" t="n">
         <v>2</v>
@@ -6349,10 +6387,10 @@
         <v>5</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="K28" s="0" t="n">
         <v>2</v>
@@ -6399,19 +6437,19 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.2602040816327"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.77551020408163"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.77551020408163"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.77551020408163"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.77551020408163"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.77551020408163"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.04591836734694"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -7059,7 +7097,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7442,9 +7480,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="0" t="s">
@@ -7568,7 +7603,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12963,7 +12998,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13393,7 +13428,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14946,7 +14981,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update baseline testing and coba2
</commit_message>
<xml_diff>
--- a/Coba2.xlsx
+++ b/Coba2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="POSresults" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,9 +19,15 @@
     <sheet name="TrainableNoTrainableTransfer" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="SkenarioPengujian" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="OhNo" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="PengujianPOS" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">OhNo!$Q$3:$R$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">OhNo!$Q$3:$R$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">OhNo!$Q$3:$R$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">OhNo!$Q$3:$R$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">OhNo!$Q$3:$R$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">OhNo!$Q$3:$R$59</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -33,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="305">
   <si>
     <t xml:space="preserve">Embedding</t>
   </si>
@@ -749,6 +755,12 @@
     <t xml:space="preserve">POS Tag</t>
   </si>
   <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Embedding (word &amp; char)</t>
   </si>
   <si>
@@ -758,9 +770,18 @@
     <t xml:space="preserve">logExM</t>
   </si>
   <si>
+    <t xml:space="preserve">← polyglot</t>
+  </si>
+  <si>
     <t xml:space="preserve">Model (WE/CE/Both)</t>
   </si>
   <si>
+    <t xml:space="preserve">← both</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trainable Embedding</t>
   </si>
   <si>
@@ -773,6 +794,12 @@
     <t xml:space="preserve">logTxM</t>
   </si>
   <si>
+    <t xml:space="preserve">← trainable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bidirectional merge (char)</t>
   </si>
   <si>
@@ -782,6 +809,15 @@
     <t xml:space="preserve">auto_script_ce.sh</t>
   </si>
   <si>
+    <t xml:space="preserve">logCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">← mul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bidirectional merge (word)</t>
   </si>
   <si>
@@ -791,18 +827,72 @@
     <t xml:space="preserve">auto_script_we.sh</t>
   </si>
   <si>
+    <t xml:space="preserve">logWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">← sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Merging layer</t>
   </si>
   <si>
     <t xml:space="preserve">← model Both</t>
   </si>
   <si>
+    <t xml:space="preserve">auto_script_bo.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">← maybe 3 (inconsistent)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Optimizer</t>
   </si>
   <si>
+    <t xml:space="preserve">auto_script_ol.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">← adam, binary_crossentropy</t>
+  </si>
+  <si>
     <t xml:space="preserve">Loss function</t>
   </si>
   <si>
+    <t xml:space="preserve">p7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">← using dev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auto_script_epoch.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logEpoch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">← still three</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dropout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auto_script_do.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">← zero dropout</t>
+  </si>
+  <si>
     <t xml:space="preserve">NER Tag</t>
   </si>
   <si>
@@ -849,6 +939,21 @@
   </si>
   <si>
     <t xml:space="preserve">0.5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id p1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rang Fasttext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rang Word2Vec</t>
   </si>
 </sst>
 </file>
@@ -1241,7 +1346,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1683,11 +1788,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="55236653"/>
-        <c:axId val="8093166"/>
+        <c:axId val="98054452"/>
+        <c:axId val="50606896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55236653"/>
+        <c:axId val="98054452"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1722,14 +1827,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8093166"/>
+        <c:crossAx val="50606896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8093166"/>
+        <c:axId val="50606896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1773,7 +1878,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55236653"/>
+        <c:crossAx val="98054452"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1810,7 +1915,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4338,11 +4443,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="86531954"/>
-        <c:axId val="88741849"/>
+        <c:axId val="50611429"/>
+        <c:axId val="14609286"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86531954"/>
+        <c:axId val="50611429"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4377,14 +4482,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88741849"/>
+        <c:crossAx val="14609286"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88741849"/>
+        <c:axId val="14609286"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4428,7 +4533,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86531954"/>
+        <c:crossAx val="50611429"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4465,7 +4570,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4701,11 +4806,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="82237733"/>
-        <c:axId val="78941774"/>
+        <c:axId val="46777520"/>
+        <c:axId val="76946684"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82237733"/>
+        <c:axId val="46777520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4740,14 +4845,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78941774"/>
+        <c:crossAx val="76946684"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78941774"/>
+        <c:axId val="76946684"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4791,7 +4896,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82237733"/>
+        <c:crossAx val="46777520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4839,9 +4944,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>561240</xdr:colOff>
+      <xdr:colOff>559440</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>21960</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4849,8 +4954,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3062160" y="361080"/>
-        <a:ext cx="5500080" cy="3237120"/>
+        <a:off x="3205080" y="361080"/>
+        <a:ext cx="5755320" cy="3235320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4869,9 +4974,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>462960</xdr:colOff>
+      <xdr:colOff>461160</xdr:colOff>
       <xdr:row>248</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4880,7 +4985,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="107280" y="36373320"/>
-        <a:ext cx="17500680" cy="4485600"/>
+        <a:ext cx="18356040" cy="4483800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4904,9 +5009,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>85680</xdr:colOff>
+      <xdr:colOff>83880</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4914,8 +5019,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2923920" y="6032880"/>
-        <a:ext cx="4133880" cy="3236400"/>
+        <a:off x="2876400" y="6032880"/>
+        <a:ext cx="4065480" cy="3234600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4940,12 +5045,12 @@
   <dimension ref="A2:S50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G39" activeCellId="0" sqref="G39"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6244,13 +6349,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:K31"/>
+  <dimension ref="A2:M38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="25" t="s">
@@ -6262,9 +6370,17 @@
         <v>237</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>239</v>
+      </c>
       <c r="B6" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>5</v>
@@ -6273,26 +6389,35 @@
         <v>15</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="M7" s="0" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>246</v>
+      </c>
       <c r="B9" s="0" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
@@ -6301,27 +6426,33 @@
         <v>3</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>245</v>
+        <v>250</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>252</v>
+      </c>
       <c r="B12" s="27" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="E12" s="27" t="n">
         <v>3</v>
@@ -6330,16 +6461,25 @@
         <v>4</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>248</v>
+        <v>255</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>258</v>
+      </c>
       <c r="B14" s="27" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="E14" s="27" t="n">
         <v>3</v>
@@ -6348,15 +6488,24 @@
         <v>4</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>251</v>
+        <v>261</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>264</v>
+      </c>
       <c r="B16" s="0" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>5</v>
@@ -6364,10 +6513,22 @@
       <c r="F16" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="H16" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>270</v>
+      </c>
       <c r="B18" s="0" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>8</v>
@@ -6375,98 +6536,144 @@
       <c r="F18" s="0" t="n">
         <v>112</v>
       </c>
+      <c r="H18" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>255</v>
+        <v>274</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="0" t="n">
-        <f aca="false">SUM(F6:F18)</f>
-        <v>143</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="25" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="28" t="s">
-        <v>257</v>
-      </c>
-      <c r="H23" s="0" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="25" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="H30" s="0" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="E25" s="0" t="n">
+      <c r="D32" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="E32" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H25" s="0" t="s">
+      <c r="H32" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="J25" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="K25" s="0" t="n">
+      <c r="J32" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="K32" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E34" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="H27" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="K27" s="0" t="n">
+      <c r="H34" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="K34" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E35" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F28" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="K28" s="0" t="n">
+      <c r="F35" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="K35" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="0" t="s">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H37" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="K30" s="0" t="n">
+      <c r="K37" s="0" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H31" s="0" t="s">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H38" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="K31" s="0" t="n">
+      <c r="K38" s="0" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6488,13 +6695,13 @@
   </sheetPr>
   <dimension ref="A1:T75"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6502,19 +6709,19 @@
         <v>148</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>261</v>
+        <v>289</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>148</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>261</v>
+        <v>289</v>
       </c>
       <c r="R1" s="0" t="s">
         <v>148</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>261</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6522,7 +6729,7 @@
         <v>227</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>150</v>
@@ -6532,7 +6739,7 @@
         <v>227</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>150</v>
@@ -6541,7 +6748,7 @@
         <v>227</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>150</v>
@@ -6551,19 +6758,19 @@
         <v>227</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>150</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>263</v>
+        <v>291</v>
       </c>
       <c r="R3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -6572,7 +6779,7 @@
         <v>0.71655193056</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>0</v>
@@ -6581,7 +6788,7 @@
         <v>0.713732499255</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0</v>
@@ -6590,7 +6797,7 @@
         <v>0.71655193056</v>
       </c>
       <c r="M4" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>0</v>
@@ -6613,7 +6820,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
@@ -6622,7 +6829,7 @@
         <v>0.71089762834</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>1</v>
@@ -6631,7 +6838,7 @@
         <v>0.724932654894</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>1</v>
@@ -6640,7 +6847,7 @@
         <v>0.71089762834</v>
       </c>
       <c r="M5" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>1</v>
@@ -6655,7 +6862,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2</v>
@@ -6664,7 +6871,7 @@
         <v>0.714972940469</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>2</v>
@@ -6673,7 +6880,7 @@
         <v>0.726672667267</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>2</v>
@@ -6682,7 +6889,7 @@
         <v>0.714972940469</v>
       </c>
       <c r="M6" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="N6" s="0" t="n">
         <v>2</v>
@@ -6697,7 +6904,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>3</v>
@@ -6706,7 +6913,7 @@
         <v>0.713816771113</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>3</v>
@@ -6715,7 +6922,7 @@
         <v>0.734510625561</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>3</v>
@@ -6724,7 +6931,7 @@
         <v>0.713816771113</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="N7" s="0" t="n">
         <v>3</v>
@@ -6739,7 +6946,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>4</v>
@@ -6748,7 +6955,7 @@
         <v>0.927015891701</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>4</v>
@@ -6757,7 +6964,7 @@
         <v>0.928941786472</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>5</v>
@@ -6766,7 +6973,7 @@
         <v>0.723072307231</v>
       </c>
       <c r="M8" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="N8" s="0" t="n">
         <v>5</v>
@@ -6781,7 +6988,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>5</v>
@@ -6790,7 +6997,7 @@
         <v>0.723072307231</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>5</v>
@@ -6799,7 +7006,7 @@
         <v>0.710353081987</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>6</v>
@@ -6808,7 +7015,7 @@
         <v>0.716034637205</v>
       </c>
       <c r="M9" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>6</v>
@@ -6823,7 +7030,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>6</v>
@@ -6832,7 +7039,7 @@
         <v>0.716034637205</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>6</v>
@@ -6841,7 +7048,7 @@
         <v>0.722884386174</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>7</v>
@@ -6850,7 +7057,7 @@
         <v>0.707360861759</v>
       </c>
       <c r="M10" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>7</v>
@@ -6865,7 +7072,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>7</v>
@@ -6874,7 +7081,7 @@
         <v>0.707360861759</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>7</v>
@@ -6883,7 +7090,7 @@
         <v>0.722404046415</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -6892,7 +7099,7 @@
         <v>0.687386843693</v>
       </c>
       <c r="M11" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="N11" s="0" t="n">
         <v>0</v>
@@ -6915,7 +7122,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>12</v>
@@ -6924,7 +7131,7 @@
         <v>0.926826396656</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>12</v>
@@ -6933,7 +7140,7 @@
         <v>0.928053738731</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>1</v>
@@ -6942,7 +7149,7 @@
         <v>0.67438318611</v>
       </c>
       <c r="M12" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>1</v>
@@ -6957,7 +7164,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -6966,7 +7173,7 @@
         <v>0.687386843693</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>0</v>
@@ -6975,7 +7182,7 @@
         <v>0.684848484848</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>2</v>
@@ -6984,7 +7191,7 @@
         <v>0.696642685851</v>
       </c>
       <c r="M13" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="N13" s="0" t="n">
         <v>2</v>
@@ -6999,7 +7206,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -7008,7 +7215,7 @@
         <v>0.67438318611</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>1</v>
@@ -7017,7 +7224,7 @@
         <v>0.669525267994</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>3</v>
@@ -7026,7 +7233,7 @@
         <v>0.68109407875</v>
       </c>
       <c r="M14" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="N14" s="0" t="n">
         <v>3</v>
@@ -7041,7 +7248,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>2</v>
@@ -7050,7 +7257,7 @@
         <v>0.696642685851</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>2</v>
@@ -7059,7 +7266,7 @@
         <v>0.6741301059</v>
       </c>
       <c r="I15" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>5</v>
@@ -7068,7 +7275,7 @@
         <v>0.667072428484</v>
       </c>
       <c r="M15" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="N15" s="0" t="n">
         <v>5</v>
@@ -7083,7 +7290,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>3</v>
@@ -7092,7 +7299,7 @@
         <v>0.68109407875</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>3</v>
@@ -7101,7 +7308,7 @@
         <v>0.702018680325</v>
       </c>
       <c r="I16" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>6</v>
@@ -7110,7 +7317,7 @@
         <v>0.683000604961</v>
       </c>
       <c r="M16" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="N16" s="0" t="n">
         <v>6</v>
@@ -7125,7 +7332,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>4</v>
@@ -7134,7 +7341,7 @@
         <v>0.920919269299</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>4</v>
@@ -7143,7 +7350,7 @@
         <v>0.923240434577</v>
       </c>
       <c r="I17" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>7</v>
@@ -7152,7 +7359,7 @@
         <v>0.649058894961</v>
       </c>
       <c r="M17" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="N17" s="0" t="n">
         <v>7</v>
@@ -7167,7 +7374,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>5</v>
@@ -7176,7 +7383,7 @@
         <v>0.667072428484</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>5</v>
@@ -7185,7 +7392,7 @@
         <v>0.681359044995</v>
       </c>
       <c r="I18" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>0</v>
@@ -7194,7 +7401,7 @@
         <v>0.637457574823</v>
       </c>
       <c r="M18" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>0</v>
@@ -7217,7 +7424,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6</v>
@@ -7226,7 +7433,7 @@
         <v>0.683000604961</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>6</v>
@@ -7235,7 +7442,7 @@
         <v>0.692307692308</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>1</v>
@@ -7244,7 +7451,7 @@
         <v>0.620174346202</v>
       </c>
       <c r="M19" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="N19" s="0" t="n">
         <v>1</v>
@@ -7259,7 +7466,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>7</v>
@@ -7268,7 +7475,7 @@
         <v>0.649058894961</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>7</v>
@@ -7277,7 +7484,7 @@
         <v>0.655677655678</v>
       </c>
       <c r="I20" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>2</v>
@@ -7286,7 +7493,7 @@
         <v>0.618844984802</v>
       </c>
       <c r="M20" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="N20" s="0" t="n">
         <v>2</v>
@@ -7301,7 +7508,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>12</v>
@@ -7310,7 +7517,7 @@
         <v>0.921888816837</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>12</v>
@@ -7319,7 +7526,7 @@
         <v>0.919853635505</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>3</v>
@@ -7328,7 +7535,7 @@
         <v>0.660741648789</v>
       </c>
       <c r="M21" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="N21" s="0" t="n">
         <v>3</v>
@@ -7343,7 +7550,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -7352,7 +7559,7 @@
         <v>0.637457574823</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>0</v>
@@ -7361,7 +7568,7 @@
         <v>0.630734680783</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>5</v>
@@ -7370,7 +7577,7 @@
         <v>0.591229684146</v>
       </c>
       <c r="M22" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>5</v>
@@ -7385,7 +7592,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>
@@ -7394,7 +7601,7 @@
         <v>0.620174346202</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>1</v>
@@ -7403,7 +7610,7 @@
         <v>0.620092735703</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="J23" s="0" t="n">
         <v>6</v>
@@ -7412,7 +7619,7 @@
         <v>0.620440156768</v>
       </c>
       <c r="M23" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="N23" s="0" t="n">
         <v>6</v>
@@ -7427,7 +7634,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>2</v>
@@ -7436,7 +7643,7 @@
         <v>0.618844984802</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>2</v>
@@ -7445,7 +7652,7 @@
         <v>0.604881062712</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>7</v>
@@ -7454,7 +7661,7 @@
         <v>0.59680393362</v>
       </c>
       <c r="M24" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="N24" s="0" t="n">
         <v>7</v>
@@ -7469,7 +7676,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>3</v>
@@ -7478,7 +7685,7 @@
         <v>0.660741648789</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>3</v>
@@ -7487,7 +7694,7 @@
         <v>0.646946564885</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>0</v>
@@ -7496,7 +7703,7 @@
         <v>0.592405063291</v>
       </c>
       <c r="M25" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="N25" s="0" t="n">
         <v>0</v>
@@ -7519,7 +7726,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>4</v>
@@ -7528,7 +7735,7 @@
         <v>0.909959313639</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>4</v>
@@ -7537,7 +7744,7 @@
         <v>0.908092792633</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>1</v>
@@ -7546,7 +7753,7 @@
         <v>0.53618628068</v>
       </c>
       <c r="M26" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="N26" s="0" t="n">
         <v>1</v>
@@ -7561,7 +7768,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>5</v>
@@ -7570,7 +7777,7 @@
         <v>0.591229684146</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>5</v>
@@ -7579,7 +7786,7 @@
         <v>0.596347607053</v>
       </c>
       <c r="I27" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>2</v>
@@ -7588,7 +7795,7 @@
         <v>0.550815558344</v>
       </c>
       <c r="M27" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="N27" s="0" t="n">
         <v>2</v>
@@ -7603,7 +7810,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>6</v>
@@ -7612,7 +7819,7 @@
         <v>0.620440156768</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>6</v>
@@ -7621,7 +7828,7 @@
         <v>0.627998785302</v>
       </c>
       <c r="I28" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="J28" s="0" t="n">
         <v>3</v>
@@ -7630,7 +7837,7 @@
         <v>0.583968302347</v>
       </c>
       <c r="M28" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="N28" s="0" t="n">
         <v>3</v>
@@ -7645,7 +7852,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>7</v>
@@ -7654,7 +7861,7 @@
         <v>0.59680393362</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>7</v>
@@ -7663,7 +7870,7 @@
         <v>0.598956735195</v>
       </c>
       <c r="I29" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>5</v>
@@ -7672,7 +7879,7 @@
         <v>0.531849103278</v>
       </c>
       <c r="M29" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="N29" s="0" t="n">
         <v>5</v>
@@ -7687,7 +7894,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>12</v>
@@ -7696,7 +7903,7 @@
         <v>0.904283009938</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>12</v>
@@ -7705,7 +7912,7 @@
         <v>0.904539267326</v>
       </c>
       <c r="I30" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>6</v>
@@ -7714,7 +7921,7 @@
         <v>0.461977186312</v>
       </c>
       <c r="M30" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="N30" s="0" t="n">
         <v>6</v>
@@ -7729,7 +7936,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0</v>
@@ -7738,7 +7945,7 @@
         <v>0.592405063291</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>0</v>
@@ -7747,7 +7954,7 @@
         <v>0.591849935317</v>
       </c>
       <c r="I31" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="J31" s="0" t="n">
         <v>7</v>
@@ -7756,7 +7963,7 @@
         <v>0.564749307905</v>
       </c>
       <c r="M31" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="N31" s="0" t="n">
         <v>7</v>
@@ -7771,7 +7978,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -7780,7 +7987,7 @@
         <v>0.53618628068</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>1</v>
@@ -7789,7 +7996,7 @@
         <v>0.555413196669</v>
       </c>
       <c r="I32" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="J32" s="0" t="n">
         <v>0</v>
@@ -7798,7 +8005,7 @@
         <v>0.472800537273</v>
       </c>
       <c r="M32" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="N32" s="0" t="n">
         <v>0</v>
@@ -7821,7 +8028,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>2</v>
@@ -7830,7 +8037,7 @@
         <v>0.550815558344</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>2</v>
@@ -7839,7 +8046,7 @@
         <v>0.575385583884</v>
       </c>
       <c r="I33" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>1</v>
@@ -7848,7 +8055,7 @@
         <v>0.434473854099</v>
       </c>
       <c r="M33" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="N33" s="0" t="n">
         <v>1</v>
@@ -7863,7 +8070,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>3</v>
@@ -7872,7 +8079,7 @@
         <v>0.583968302347</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>3</v>
@@ -7881,7 +8088,7 @@
         <v>0.57501569366</v>
       </c>
       <c r="I34" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>2</v>
@@ -7890,7 +8097,7 @@
         <v>0.510901399284</v>
       </c>
       <c r="M34" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="N34" s="0" t="n">
         <v>2</v>
@@ -7905,7 +8112,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>4</v>
@@ -7914,7 +8121,7 @@
         <v>0.890085824208</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>4</v>
@@ -7923,7 +8130,7 @@
         <v>0.894602458286</v>
       </c>
       <c r="I35" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="J35" s="0" t="n">
         <v>3</v>
@@ -7932,7 +8139,7 @@
         <v>0.474908200734</v>
       </c>
       <c r="M35" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="N35" s="0" t="n">
         <v>3</v>
@@ -7947,7 +8154,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>5</v>
@@ -7956,7 +8163,7 @@
         <v>0.531849103278</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>5</v>
@@ -7965,7 +8172,7 @@
         <v>0.55317769131</v>
       </c>
       <c r="I36" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="J36" s="0" t="n">
         <v>5</v>
@@ -7974,7 +8181,7 @@
         <v>0.486912645853</v>
       </c>
       <c r="M36" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="N36" s="0" t="n">
         <v>5</v>
@@ -7989,7 +8196,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>6</v>
@@ -7998,7 +8205,7 @@
         <v>0.461977186312</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>6</v>
@@ -8007,7 +8214,7 @@
         <v>0.507824976046</v>
       </c>
       <c r="I37" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="J37" s="0" t="n">
         <v>6</v>
@@ -8016,7 +8223,7 @@
         <v>0.368553459119</v>
       </c>
       <c r="M37" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="N37" s="0" t="n">
         <v>6</v>
@@ -8031,7 +8238,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>7</v>
@@ -8040,7 +8247,7 @@
         <v>0.564749307905</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>7</v>
@@ -8049,7 +8256,7 @@
         <v>0.551767676768</v>
       </c>
       <c r="I38" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="J38" s="0" t="n">
         <v>7</v>
@@ -8058,7 +8265,7 @@
         <v>0.476656872347</v>
       </c>
       <c r="M38" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="N38" s="0" t="n">
         <v>7</v>
@@ -8073,7 +8280,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>12</v>
@@ -8082,7 +8289,7 @@
         <v>0.895278665247</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>12</v>
@@ -8091,7 +8298,7 @@
         <v>0.894328216678</v>
       </c>
       <c r="I39" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="J39" s="0" t="n">
         <v>0</v>
@@ -8100,7 +8307,7 @@
         <v>0.260103312063</v>
       </c>
       <c r="M39" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="N39" s="0" t="n">
         <v>0</v>
@@ -8123,7 +8330,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0</v>
@@ -8132,7 +8339,7 @@
         <v>0.472800537273</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>0</v>
@@ -8141,7 +8348,7 @@
         <v>0.491110365649</v>
       </c>
       <c r="I40" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="J40" s="0" t="n">
         <v>1</v>
@@ -8150,7 +8357,7 @@
         <v>0.420795533845</v>
       </c>
       <c r="M40" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="N40" s="0" t="n">
         <v>1</v>
@@ -8165,7 +8372,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
@@ -8174,7 +8381,7 @@
         <v>0.434473854099</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>1</v>
@@ -8183,7 +8390,7 @@
         <v>0.518118245391</v>
       </c>
       <c r="I41" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="J41" s="0" t="n">
         <v>2</v>
@@ -8192,7 +8399,7 @@
         <v>0.377164849262</v>
       </c>
       <c r="M41" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="N41" s="0" t="n">
         <v>2</v>
@@ -8207,7 +8414,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>2</v>
@@ -8216,7 +8423,7 @@
         <v>0.510901399284</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>2</v>
@@ -8225,7 +8432,7 @@
         <v>0.568085797855</v>
       </c>
       <c r="I42" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="J42" s="0" t="n">
         <v>3</v>
@@ -8234,7 +8441,7 @@
         <v>0.361445783133</v>
       </c>
       <c r="M42" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="N42" s="0" t="n">
         <v>3</v>
@@ -8249,7 +8456,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>3</v>
@@ -8258,7 +8465,7 @@
         <v>0.474908200734</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>3</v>
@@ -8267,7 +8474,7 @@
         <v>0.467459762071</v>
       </c>
       <c r="I43" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="J43" s="0" t="n">
         <v>5</v>
@@ -8276,7 +8483,7 @@
         <v>0.3192550715</v>
       </c>
       <c r="M43" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="N43" s="0" t="n">
         <v>5</v>
@@ -8291,7 +8498,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>4</v>
@@ -8300,7 +8507,7 @@
         <v>0.884699745095</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>4</v>
@@ -8309,7 +8516,7 @@
         <v>0.88298567778</v>
       </c>
       <c r="I44" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="J44" s="0" t="n">
         <v>6</v>
@@ -8318,7 +8525,7 @@
         <v>0.295857988166</v>
       </c>
       <c r="M44" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="N44" s="0" t="n">
         <v>6</v>
@@ -8333,7 +8540,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>5</v>
@@ -8342,7 +8549,7 @@
         <v>0.486912645853</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="F45" s="0" t="n">
         <v>5</v>
@@ -8351,7 +8558,7 @@
         <v>0.473755047106</v>
       </c>
       <c r="I45" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="J45" s="0" t="n">
         <v>7</v>
@@ -8360,7 +8567,7 @@
         <v>0.345389377647</v>
       </c>
       <c r="M45" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="N45" s="0" t="n">
         <v>7</v>
@@ -8375,7 +8582,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>6</v>
@@ -8384,7 +8591,7 @@
         <v>0.368553459119</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="F46" s="0" t="n">
         <v>6</v>
@@ -8393,7 +8600,7 @@
         <v>0.465788628333</v>
       </c>
       <c r="I46" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="J46" s="0" t="n">
         <v>0</v>
@@ -8402,7 +8609,7 @@
         <v>0.250269687163</v>
       </c>
       <c r="M46" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="N46" s="0" t="n">
         <v>0</v>
@@ -8425,7 +8632,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>7</v>
@@ -8434,7 +8641,7 @@
         <v>0.476656872347</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="F47" s="0" t="n">
         <v>7</v>
@@ -8443,7 +8650,7 @@
         <v>0.452945159106</v>
       </c>
       <c r="I47" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="J47" s="0" t="n">
         <v>1</v>
@@ -8452,7 +8659,7 @@
         <v>0.324441240087</v>
       </c>
       <c r="M47" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="N47" s="0" t="n">
         <v>1</v>
@@ -8467,7 +8674,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>12</v>
@@ -8476,7 +8683,7 @@
         <v>0.878253172027</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="F48" s="0" t="n">
         <v>12</v>
@@ -8485,7 +8692,7 @@
         <v>0.86400661079</v>
       </c>
       <c r="I48" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="J48" s="0" t="n">
         <v>2</v>
@@ -8494,7 +8701,7 @@
         <v>0.266412940057</v>
       </c>
       <c r="M48" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="N48" s="0" t="n">
         <v>2</v>
@@ -8509,7 +8716,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0</v>
@@ -8518,7 +8725,7 @@
         <v>0.260103312063</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="F49" s="0" t="n">
         <v>0</v>
@@ -8527,7 +8734,7 @@
         <v>0.300450266066</v>
       </c>
       <c r="I49" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="J49" s="0" t="n">
         <v>3</v>
@@ -8536,7 +8743,7 @@
         <v>0.296150049358</v>
       </c>
       <c r="M49" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="N49" s="0" t="n">
         <v>3</v>
@@ -8551,7 +8758,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1</v>
@@ -8560,7 +8767,7 @@
         <v>0.420795533845</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="F50" s="0" t="n">
         <v>1</v>
@@ -8569,7 +8776,7 @@
         <v>0.352982211371</v>
       </c>
       <c r="I50" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="J50" s="0" t="n">
         <v>5</v>
@@ -8578,7 +8785,7 @@
         <v>0.22844126261</v>
       </c>
       <c r="M50" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="N50" s="0" t="n">
         <v>5</v>
@@ -8593,7 +8800,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>2</v>
@@ -8602,7 +8809,7 @@
         <v>0.377164849262</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>2</v>
@@ -8611,7 +8818,7 @@
         <v>0.333449356074</v>
       </c>
       <c r="I51" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="J51" s="0" t="n">
         <v>6</v>
@@ -8620,7 +8827,7 @@
         <v>0.292492687683</v>
       </c>
       <c r="M51" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="N51" s="0" t="n">
         <v>6</v>
@@ -8635,7 +8842,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>3</v>
@@ -8644,7 +8851,7 @@
         <v>0.361445783133</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="F52" s="0" t="n">
         <v>3</v>
@@ -8653,7 +8860,7 @@
         <v>0.358992060753</v>
       </c>
       <c r="I52" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="J52" s="0" t="n">
         <v>7</v>
@@ -8662,7 +8869,7 @@
         <v>0.23265940902</v>
       </c>
       <c r="M52" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="N52" s="0" t="n">
         <v>7</v>
@@ -8677,7 +8884,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>4</v>
@@ -8686,7 +8893,7 @@
         <v>0.867099541312</v>
       </c>
       <c r="E53" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="F53" s="0" t="n">
         <v>4</v>
@@ -8695,7 +8902,7 @@
         <v>0.857176791971</v>
       </c>
       <c r="I53" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="J53" s="0" t="n">
         <v>0</v>
@@ -8704,7 +8911,7 @@
         <v>0.306393244873</v>
       </c>
       <c r="M53" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="N53" s="0" t="n">
         <v>0</v>
@@ -8727,7 +8934,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>5</v>
@@ -8736,7 +8943,7 @@
         <v>0.3192550715</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="F54" s="0" t="n">
         <v>5</v>
@@ -8745,7 +8952,7 @@
         <v>0.307990690458</v>
       </c>
       <c r="I54" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="J54" s="0" t="n">
         <v>1</v>
@@ -8754,7 +8961,7 @@
         <v>0.171532846715</v>
       </c>
       <c r="M54" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="N54" s="0" t="n">
         <v>1</v>
@@ -8769,7 +8976,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>6</v>
@@ -8778,7 +8985,7 @@
         <v>0.295857988166</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="F55" s="0" t="n">
         <v>6</v>
@@ -8787,7 +8994,7 @@
         <v>0.302325581395</v>
       </c>
       <c r="I55" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="J55" s="0" t="n">
         <v>2</v>
@@ -8796,7 +9003,7 @@
         <v>0.221264367816</v>
       </c>
       <c r="M55" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="N55" s="0" t="n">
         <v>2</v>
@@ -8811,7 +9018,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>7</v>
@@ -8820,7 +9027,7 @@
         <v>0.345389377647</v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>7</v>
@@ -8829,7 +9036,7 @@
         <v>0.318656716418</v>
       </c>
       <c r="I56" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="J56" s="0" t="n">
         <v>3</v>
@@ -8838,7 +9045,7 @@
         <v>0.301687065829</v>
       </c>
       <c r="M56" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="N56" s="0" t="n">
         <v>3</v>
@@ -8853,7 +9060,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>12</v>
@@ -8862,7 +9069,7 @@
         <v>0.850067802606</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="F57" s="0" t="n">
         <v>12</v>
@@ -8871,7 +9078,7 @@
         <v>0.840415486308</v>
       </c>
       <c r="I57" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="J57" s="0" t="n">
         <v>5</v>
@@ -8880,7 +9087,7 @@
         <v>0.210690596957</v>
       </c>
       <c r="M57" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="N57" s="0" t="n">
         <v>5</v>
@@ -8895,7 +9102,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>0</v>
@@ -8904,7 +9111,7 @@
         <v>0.250269687163</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="F58" s="0" t="n">
         <v>0</v>
@@ -8913,7 +9120,7 @@
         <v>0.229408792319</v>
       </c>
       <c r="I58" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="J58" s="0" t="n">
         <v>6</v>
@@ -8922,7 +9129,7 @@
         <v>0.196775255018</v>
       </c>
       <c r="M58" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="N58" s="0" t="n">
         <v>6</v>
@@ -8937,7 +9144,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>1</v>
@@ -8946,7 +9153,7 @@
         <v>0.324441240087</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="F59" s="0" t="n">
         <v>1</v>
@@ -8955,7 +9162,7 @@
         <v>0.267498885421</v>
       </c>
       <c r="I59" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="J59" s="0" t="n">
         <v>7</v>
@@ -8964,7 +9171,7 @@
         <v>0.156965336821</v>
       </c>
       <c r="M59" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="N59" s="0" t="n">
         <v>7</v>
@@ -8979,7 +9186,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>2</v>
@@ -8988,7 +9195,7 @@
         <v>0.266412940057</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="F60" s="0" t="n">
         <v>2</v>
@@ -8999,7 +9206,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>3</v>
@@ -9008,7 +9215,7 @@
         <v>0.296150049358</v>
       </c>
       <c r="E61" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="F61" s="0" t="n">
         <v>3</v>
@@ -9019,7 +9226,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>4</v>
@@ -9028,7 +9235,7 @@
         <v>0.842689989363</v>
       </c>
       <c r="E62" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="F62" s="0" t="n">
         <v>4</v>
@@ -9039,7 +9246,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>5</v>
@@ -9048,7 +9255,7 @@
         <v>0.22844126261</v>
       </c>
       <c r="E63" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="F63" s="0" t="n">
         <v>5</v>
@@ -9059,7 +9266,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>6</v>
@@ -9068,7 +9275,7 @@
         <v>0.292492687683</v>
       </c>
       <c r="E64" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="F64" s="0" t="n">
         <v>6</v>
@@ -9079,7 +9286,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>7</v>
@@ -9088,7 +9295,7 @@
         <v>0.23265940902</v>
       </c>
       <c r="E65" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="F65" s="0" t="n">
         <v>7</v>
@@ -9099,7 +9306,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>12</v>
@@ -9108,7 +9315,7 @@
         <v>0.837181903864</v>
       </c>
       <c r="E66" s="29" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
       <c r="F66" s="0" t="n">
         <v>12</v>
@@ -9119,7 +9326,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>0</v>
@@ -9128,7 +9335,7 @@
         <v>0.306393244873</v>
       </c>
       <c r="E67" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="F67" s="0" t="n">
         <v>0</v>
@@ -9139,7 +9346,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>1</v>
@@ -9148,7 +9355,7 @@
         <v>0.171532846715</v>
       </c>
       <c r="E68" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="F68" s="0" t="n">
         <v>1</v>
@@ -9159,7 +9366,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>2</v>
@@ -9168,7 +9375,7 @@
         <v>0.221264367816</v>
       </c>
       <c r="E69" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="F69" s="0" t="n">
         <v>2</v>
@@ -9179,7 +9386,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>3</v>
@@ -9188,7 +9395,7 @@
         <v>0.301687065829</v>
       </c>
       <c r="E70" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="F70" s="0" t="n">
         <v>3</v>
@@ -9199,7 +9406,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>4</v>
@@ -9208,7 +9415,7 @@
         <v>0.855546687949</v>
       </c>
       <c r="E71" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="F71" s="0" t="n">
         <v>4</v>
@@ -9219,7 +9426,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>5</v>
@@ -9228,7 +9435,7 @@
         <v>0.210690596957</v>
       </c>
       <c r="E72" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="F72" s="0" t="n">
         <v>5</v>
@@ -9239,7 +9446,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>6</v>
@@ -9248,7 +9455,7 @@
         <v>0.196775255018</v>
       </c>
       <c r="E73" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="F73" s="0" t="n">
         <v>6</v>
@@ -9259,7 +9466,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>7</v>
@@ -9268,7 +9475,7 @@
         <v>0.156965336821</v>
       </c>
       <c r="E74" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="F74" s="0" t="n">
         <v>7</v>
@@ -9279,7 +9486,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>12</v>
@@ -9288,7 +9495,7 @@
         <v>0.827683615819</v>
       </c>
       <c r="E75" s="29" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="F75" s="0" t="n">
         <v>12</v>
@@ -9307,6 +9514,65 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:E5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -9324,19 +9590,19 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.44897959183673"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.83163265306122"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.83163265306122"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.83163265306122"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.83163265306122"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="7.83163265306122"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="7.96428571428571"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -9984,7 +10250,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="6.88265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10368,7 +10634,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10492,6 +10758,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -15884,9 +16153,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -16314,9 +16580,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -17867,9 +18130,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>